<commit_message>
Update NaN related to numpy version. Update plots and tables
</commit_message>
<xml_diff>
--- a/conclusions/tables/gr4j_hbv_statistics.xlsx
+++ b/conclusions/tables/gr4j_hbv_statistics.xlsx
@@ -477,25 +477,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3577775531942567</v>
+        <v>0.36</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3442058272739959</v>
+        <v>0.34</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7093931457217669</v>
+        <v>0.71</v>
       </c>
       <c r="E2" t="n">
-        <v>1.200965863381587</v>
+        <v>1.2</v>
       </c>
       <c r="F2" t="n">
-        <v>1.304886704647785</v>
+        <v>1.31</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6041403434683817</v>
+        <v>0.61</v>
       </c>
       <c r="H2" t="n">
-        <v>26.67553416359749</v>
+        <v>26.73</v>
       </c>
     </row>
     <row r="3">
@@ -505,25 +505,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4430850206686476</v>
+        <v>0.44</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4599459051447959</v>
+        <v>0.46</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7336267563451166</v>
+        <v>0.73</v>
       </c>
       <c r="E3" t="n">
-        <v>1.219051493362542</v>
+        <v>1.22</v>
       </c>
       <c r="F3" t="n">
-        <v>1.036671319366357</v>
+        <v>1.04</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5589187946902365</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H3" t="n">
-        <v>-32.8110977946282</v>
+        <v>-32.81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update tables, plots and some code in two chapters
</commit_message>
<xml_diff>
--- a/conclusions/tables/gr4j_hbv_statistics.xlsx
+++ b/conclusions/tables/gr4j_hbv_statistics.xlsx
@@ -489,13 +489,13 @@
         <v>1.2</v>
       </c>
       <c r="F2" t="n">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="G2" t="n">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
       <c r="H2" t="n">
-        <v>26.73</v>
+        <v>26.68</v>
       </c>
     </row>
     <row r="3">

</xml_diff>